<commit_message>
Added PnP Dire Rat.
Added PnP Dire Rat.
</commit_message>
<xml_diff>
--- a/nwnds_notes/AnimalCompanionWorksheet.xlsx
+++ b/nwnds_notes/AnimalCompanionWorksheet.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785"/>
+    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Erdlu_AC" sheetId="1" r:id="rId1"/>
+    <sheet name="Dire Rat AC" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="79">
   <si>
     <t>Progression:</t>
   </si>
@@ -233,6 +234,24 @@
   </si>
   <si>
     <t>Armor Skin</t>
+  </si>
+  <si>
+    <t>Alterness</t>
+  </si>
+  <si>
+    <t>WF(Creature)</t>
+  </si>
+  <si>
+    <t>Spr Attack</t>
+  </si>
+  <si>
+    <t>Iron Will</t>
+  </si>
+  <si>
+    <t>EWF (Creature)</t>
+  </si>
+  <si>
+    <t>Epic Prowess</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1533,4 +1552,471 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A4:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2">
+        <f>SUM(G6+2)</f>
+        <v>3</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8:G12" si="0">SUM(G7+2)</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2">
+        <f>SUM(G12+2)</f>
+        <v>15</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17:G22" si="1">SUM(G16+2)</f>
+        <v>17</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Kivit Animal Companion.
Added Kivit Animal Companion & re-vamped the rest of the Animal Companions.
</commit_message>
<xml_diff>
--- a/nwnds_notes/AnimalCompanionWorksheet.xlsx
+++ b/nwnds_notes/AnimalCompanionWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785"/>
+    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="792" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Boneclaw_AC" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="101">
   <si>
     <t>Progression:</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>Track</t>
+  </si>
+  <si>
+    <t>Feats: Low-Light Vision, Weapon Focus (Creature)*, Weapon Finesse</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1688,7 +1691,7 @@
   <dimension ref="A4:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2716,7 +2719,7 @@
   <dimension ref="A4:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3231,7 +3234,7 @@
   <dimension ref="A4:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3566,7 +3569,7 @@
         <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>23</v>
@@ -3596,7 +3599,7 @@
         <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>23</v>
@@ -3740,7 +3743,7 @@
   <dimension ref="A4:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4254,8 +4257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4764,7 +4767,7 @@
   <dimension ref="A4:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5276,10 +5279,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:I22"/>
+  <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5294,6 +5297,11 @@
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Added kes'trekel animal companion
Added kes'trekel animal companion
</commit_message>
<xml_diff>
--- a/nwnds_notes/AnimalCompanionWorksheet.xlsx
+++ b/nwnds_notes/AnimalCompanionWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="792" activeTab="6"/>
+    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="792" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Boneclaw_AC" sheetId="4" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Kivit_AC" sheetId="3" r:id="rId7"/>
     <sheet name="Sand Howler_AC" sheetId="8" r:id="rId8"/>
     <sheet name="Z'tal_AC" sheetId="9" r:id="rId9"/>
+    <sheet name="Kestrekel_AC" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="103">
   <si>
     <t>Progression:</t>
   </si>
@@ -325,6 +326,12 @@
   </si>
   <si>
     <t>Feats: Low-Light Vision, Weapon Focus (Creature)*, Weapon Finesse</t>
+  </si>
+  <si>
+    <t>Spring Attack*</t>
+  </si>
+  <si>
+    <t>Improved Critical</t>
   </si>
 </sst>
 </file>
@@ -1686,6 +1693,515 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A4:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2">
+        <f>SUM(G6+2)</f>
+        <v>3</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8:G12" si="0">SUM(G7+2)</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2">
+        <f>SUM(G12+2)</f>
+        <v>15</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17:G22" si="1">SUM(G16+2)</f>
+        <v>17</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:I22"/>
@@ -4257,7 +4773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Notes for owl animal companion
Notes for owl animal companion.
</commit_message>
<xml_diff>
--- a/nwnds_notes/AnimalCompanionWorksheet.xlsx
+++ b/nwnds_notes/AnimalCompanionWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="792" activeTab="9"/>
+    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="792" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Boneclaw_AC" sheetId="4" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Sand Howler_AC" sheetId="8" r:id="rId8"/>
     <sheet name="Z'tal_AC" sheetId="9" r:id="rId9"/>
     <sheet name="Kestrekel_AC" sheetId="10" r:id="rId10"/>
+    <sheet name="Owl_AC" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="104">
   <si>
     <t>Progression:</t>
   </si>
@@ -332,6 +333,9 @@
   </si>
   <si>
     <t>Improved Critical</t>
+  </si>
+  <si>
+    <t>Alertness*</t>
   </si>
 </sst>
 </file>
@@ -1697,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2195,6 +2199,530 @@
       <c r="I22" s="3" t="s">
         <v>23</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A4:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2">
+        <f>SUM(G6+2)</f>
+        <v>3</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8:G12" si="0">SUM(G7+2)</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2">
+        <f>SUM(G12+2)</f>
+        <v>15</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17:G22" si="1">SUM(G16+2)</f>
+        <v>17</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added owl animal companion.
Added owl animal companion.
</commit_message>
<xml_diff>
--- a/nwnds_notes/AnimalCompanionWorksheet.xlsx
+++ b/nwnds_notes/AnimalCompanionWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="792" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="843" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Boneclaw_AC" sheetId="4" r:id="rId1"/>
@@ -2210,7 +2210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed owl PnP animal companion.
Fixed owl PnP animal companion.
</commit_message>
<xml_diff>
--- a/nwnds_notes/AnimalCompanionWorksheet.xlsx
+++ b/nwnds_notes/AnimalCompanionWorksheet.xlsx
@@ -2210,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>